<commit_message>
feat: implement sector analysis with metrics calculation and database storage
</commit_message>
<xml_diff>
--- a/finfun-ts/backend/src/portfolio_sector_normalization.xlsx
+++ b/finfun-ts/backend/src/portfolio_sector_normalization.xlsx
@@ -445,10 +445,10 @@
         <v>8.254</v>
       </c>
       <c r="F2">
-        <v>18.301338</v>
+        <v>19.266619</v>
       </c>
       <c r="G2">
-        <v>0.20801738710456422</v>
+        <v>0.023426486394750368</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         <v>Technology</v>
       </c>
       <c r="C3">
-        <v>0.005</v>
+        <v>0.0050999997</v>
       </c>
       <c r="D3">
         <v>0.24301</v>
@@ -468,10 +468,10 @@
         <v>146.994</v>
       </c>
       <c r="F3">
-        <v>24.892899</v>
+        <v>24.338146</v>
       </c>
       <c r="G3">
-        <v>0.20469050365244137</v>
+        <v>0.0007899811224648264</v>
       </c>
     </row>
     <row r="4">
@@ -491,10 +491,10 @@
         <v>26.763</v>
       </c>
       <c r="F4">
-        <v>25.181818</v>
+        <v>25.276854</v>
       </c>
       <c r="G4">
-        <v>0.14011148452578578</v>
+        <v>0.005807474659536062</v>
       </c>
     </row>
     <row r="5">
@@ -505,7 +505,7 @@
         <v>Technology</v>
       </c>
       <c r="C5">
-        <v>0.0072000003</v>
+        <v>0.0073</v>
       </c>
       <c r="D5">
         <v>0.35789</v>
@@ -514,10 +514,10 @@
         <v>32.626</v>
       </c>
       <c r="F5">
-        <v>30.646824</v>
+        <v>30.535118</v>
       </c>
       <c r="G5">
-        <v>0.021735881285363523</v>
+        <v>0.008136970526567382</v>
       </c>
     </row>
   </sheetData>
@@ -583,10 +583,10 @@
         <v>8.254</v>
       </c>
       <c r="F2">
-        <v>18.301338</v>
+        <v>19.266619</v>
       </c>
       <c r="G2">
-        <v>0.20801738710456422</v>
+        <v>0.023426486394750368</v>
       </c>
     </row>
     <row r="3">
@@ -597,7 +597,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C3">
-        <v>0.005</v>
+        <v>0.0049</v>
       </c>
       <c r="D3">
         <v>0.30857</v>
@@ -606,10 +606,10 @@
         <v>8.254</v>
       </c>
       <c r="F3">
-        <v>18.47151</v>
+        <v>19.435196</v>
       </c>
       <c r="G3">
-        <v>0.20785816962146622</v>
+        <v>0.023494077359232035</v>
       </c>
     </row>
     <row r="4">
@@ -620,7 +620,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C4">
-        <v>0.0396</v>
+        <v>0.0404</v>
       </c>
       <c r="D4">
         <v>0.096429996</v>
@@ -629,10 +629,10 @@
         <v>119.246</v>
       </c>
       <c r="F4">
-        <v>12.401786</v>
+        <v>12.234955</v>
       </c>
       <c r="G4">
-        <v>0.043058904581467446</v>
+        <v>0.010959942259112204</v>
       </c>
     </row>
     <row r="5">
@@ -652,10 +652,10 @@
         <v>465.632</v>
       </c>
       <c r="F5">
-        <v>11.835942</v>
+        <v>11.503075</v>
       </c>
       <c r="G5">
-        <v>0.03104836864503728</v>
+        <v>0.015276398741521398</v>
       </c>
     </row>
     <row r="6">
@@ -666,7 +666,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C6">
-        <v>0.0372</v>
+        <v>0.0376</v>
       </c>
       <c r="D6">
         <v>0.12714</v>
@@ -675,10 +675,10 @@
         <v>113.542</v>
       </c>
       <c r="F6">
-        <v>8.12557</v>
+        <v>7.943082</v>
       </c>
       <c r="G6">
-        <v>0.21452218053409838</v>
+        <v>0.012469486233323755</v>
       </c>
     </row>
     <row r="7">
@@ -698,10 +698,10 @@
         <v>6.278</v>
       </c>
       <c r="F7">
-        <v>115.26966</v>
+        <v>114.134834</v>
       </c>
       <c r="G7">
-        <v>0.04676066807591348</v>
+        <v>0.016341055995351877</v>
       </c>
     </row>
     <row r="8">
@@ -712,7 +712,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C8">
-        <v>0.0050999997</v>
+        <v>0.005</v>
       </c>
       <c r="D8">
         <v>0.15021</v>
@@ -721,10 +721,10 @@
         <v>34.732</v>
       </c>
       <c r="F8">
-        <v>17.810081</v>
+        <v>17.287224</v>
       </c>
       <c r="G8">
-        <v>0.09839762611275972</v>
+        <v>0.026088105144970536</v>
       </c>
     </row>
     <row r="9">
@@ -735,7 +735,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C9">
-        <v>0.0097</v>
+        <v>0.0098</v>
       </c>
       <c r="D9">
         <v>0.1158</v>
@@ -744,10 +744,10 @@
         <v>68.321</v>
       </c>
       <c r="F9">
-        <v>15.147453</v>
+        <v>14.699733</v>
       </c>
       <c r="G9">
-        <v>0.038134150493701086</v>
+        <v>0.009215757137694345</v>
       </c>
     </row>
     <row r="10">
@@ -758,7 +758,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C10">
-        <v>0.0105</v>
+        <v>0.0106</v>
       </c>
       <c r="D10">
         <v>0.1158</v>
@@ -767,10 +767,10 @@
         <v>68.321</v>
       </c>
       <c r="F10">
-        <v>22.195745</v>
+        <v>21.459576</v>
       </c>
       <c r="G10">
-        <v>0.051636363636363695</v>
+        <v>0.0111764705882353</v>
       </c>
     </row>
     <row r="11">
@@ -781,7 +781,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C11">
-        <v>0.051799998</v>
+        <v>0.0544</v>
       </c>
       <c r="D11">
         <v>0.05485</v>
@@ -790,10 +790,10 @@
         <v>113.87</v>
       </c>
       <c r="F11">
-        <v>9.167273</v>
+        <v>8.801818</v>
       </c>
       <c r="G11">
-        <v>0.23721633888048402</v>
+        <v>0.004319210201563161</v>
       </c>
     </row>
     <row r="12">
@@ -813,10 +813,10 @@
         <v>393.218</v>
       </c>
       <c r="F12">
-        <v>60.45041</v>
+        <v>59.92975</v>
       </c>
       <c r="G12">
-        <v>0.0726465927099842</v>
+        <v>0.000895563516120112</v>
       </c>
     </row>
     <row r="13">
@@ -836,10 +836,10 @@
         <v>26.763</v>
       </c>
       <c r="F13">
-        <v>25.181818</v>
+        <v>25.276854</v>
       </c>
       <c r="G13">
-        <v>0.14011148452578578</v>
+        <v>0.005807474659536062</v>
       </c>
     </row>
     <row r="14">
@@ -859,10 +859,10 @@
         <v>72.513</v>
       </c>
       <c r="F14">
-        <v>50.126995</v>
+        <v>50.269135</v>
       </c>
       <c r="G14">
-        <v>0.003744254074383634</v>
+        <v>0.0027861524743400964</v>
       </c>
     </row>
     <row r="15">
@@ -873,7 +873,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C15">
-        <v>0.0070999996</v>
+        <v>0.0072000003</v>
       </c>
       <c r="D15">
         <v>0.04743</v>
@@ -882,10 +882,10 @@
         <v>32.188</v>
       </c>
       <c r="F15">
-        <v>26.726416</v>
+        <v>26.17453</v>
       </c>
       <c r="G15">
-        <v>0.07689801238188344</v>
+        <v>0.022030313711667252</v>
       </c>
     </row>
     <row r="16">
@@ -896,7 +896,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C16">
-        <v>0.0061000003</v>
+        <v>0.0062</v>
       </c>
       <c r="D16">
         <v>0.04743</v>
@@ -905,10 +905,10 @@
         <v>32.188</v>
       </c>
       <c r="F16">
-        <v>39.97561</v>
+        <v>39.091465</v>
       </c>
       <c r="G16">
-        <v>0.07007092198581558</v>
+        <v>0.006816421378776107</v>
       </c>
     </row>
     <row r="17">
@@ -919,7 +919,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C17">
-        <v>0.0364</v>
+        <v>0.0381</v>
       </c>
       <c r="D17">
         <v>0.09205</v>
@@ -928,10 +928,10 @@
         <v>129.051</v>
       </c>
       <c r="F17">
-        <v>8.806712</v>
+        <v>8.503472</v>
       </c>
       <c r="G17">
-        <v>0.28887850467289716</v>
+        <v>0.0032276051820767683</v>
       </c>
     </row>
     <row r="18">
@@ -942,7 +942,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C18">
-        <v>0.017</v>
+        <v>0.0168</v>
       </c>
       <c r="D18">
         <v>-0.19094999</v>
@@ -951,10 +951,10 @@
         <v>91.724</v>
       </c>
       <c r="F18">
-        <v>7.2822084</v>
+        <v>7.285276</v>
       </c>
       <c r="G18">
-        <v>0.09042145593869742</v>
+        <v>0.00461022632020115</v>
       </c>
     </row>
     <row r="19">
@@ -965,7 +965,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C19">
-        <v>0.014400001</v>
+        <v>0.0146</v>
       </c>
       <c r="D19">
         <v>0.14413</v>
@@ -974,10 +974,10 @@
         <v>199.152</v>
       </c>
       <c r="F19">
-        <v>22.606373</v>
+        <v>22.547329</v>
       </c>
       <c r="G19">
-        <v>0.12759955152085067</v>
+        <v>0.006114186565314343</v>
       </c>
     </row>
     <row r="20">
@@ -997,10 +997,10 @@
         <v>192.071</v>
       </c>
       <c r="F20">
-        <v>30.293367</v>
+        <v>28.958546</v>
       </c>
       <c r="G20">
-        <v>0.013622393886535432</v>
+        <v>0.005976357267951003</v>
       </c>
     </row>
     <row r="21">
@@ -1011,7 +1011,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C21">
-        <v>0.0093</v>
+        <v>0.0095</v>
       </c>
       <c r="D21">
         <v>0.06022</v>
@@ -1020,10 +1020,10 @@
         <v>30.107</v>
       </c>
       <c r="F21">
-        <v>50.228397</v>
+        <v>48.527775</v>
       </c>
       <c r="G21">
-        <v>0.09129487966943992</v>
+        <v>0.016451895408482572</v>
       </c>
     </row>
     <row r="22">
@@ -1034,7 +1034,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C22">
-        <v>0.0612</v>
+        <v>0.0619</v>
       </c>
       <c r="D22">
         <v>0.13144</v>
@@ -1043,10 +1043,10 @@
         <v>169.089</v>
       </c>
       <c r="F22">
-        <v>9.348838</v>
+        <v>9.1712475</v>
       </c>
       <c r="G22">
-        <v>0.06630067567567569</v>
+        <v>0.010492700729927026</v>
       </c>
     </row>
     <row r="23">
@@ -1057,7 +1057,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C23">
-        <v>0.0089</v>
+        <v>0.0091</v>
       </c>
       <c r="D23">
         <v>0.09475</v>
@@ -1066,10 +1066,10 @@
         <v>39.432</v>
       </c>
       <c r="F23">
-        <v>21.817476</v>
+        <v>21.673786</v>
       </c>
       <c r="G23">
-        <v>0.052853409761443114</v>
+        <v>0.0010739216037228417</v>
       </c>
     </row>
     <row r="24">
@@ -1089,10 +1089,10 @@
         <v>106.412</v>
       </c>
       <c r="F24">
-        <v>-71</v>
+        <v>-69.26923</v>
       </c>
       <c r="G24">
-        <v>0.27322834645669286</v>
+        <v>0.000554938956714651</v>
       </c>
     </row>
     <row r="25">
@@ -1103,7 +1103,7 @@
         <v/>
       </c>
       <c r="C25">
-        <v>0.01424347820869565</v>
+        <v>0.01453913045652174</v>
       </c>
       <c r="D25">
         <v>0.06157739043478259</v>
@@ -1112,10 +1112,10 @@
         <v>109.58078260869564</v>
       </c>
       <c r="F25">
-        <v>23.068303408695655</v>
+        <v>22.822002065217397</v>
       </c>
       <c r="G25">
-        <v>0.11062263656286699</v>
+        <v>0.010417597731764565</v>
       </c>
     </row>
     <row r="26">
@@ -1126,7 +1126,7 @@
         <v/>
       </c>
       <c r="C26">
-        <v>0.017545464388223308</v>
+        <v>0.01803216302069066</v>
       </c>
       <c r="D26">
         <v>0.22940302806275004</v>
@@ -1135,10 +1135,10 @@
         <v>113.8436591848879</v>
       </c>
       <c r="F26">
-        <v>30.932727183904056</v>
+        <v>30.46340248938333</v>
       </c>
       <c r="G26">
-        <v>0.08344047820095166</v>
+        <v>0.007663708478974685</v>
       </c>
     </row>
     <row r="27">
@@ -1220,7 +1220,7 @@
         <v>GOOGL</v>
       </c>
       <c r="B2">
-        <v>96.12765454093841</v>
+        <v>96.05319707489454</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -1237,10 +1237,10 @@
         <v>50</v>
       </c>
       <c r="C3">
-        <v>93.65082970356796</v>
+        <v>50</v>
       </c>
       <c r="D3">
-        <v>70.40926293568634</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -1248,13 +1248,13 @@
         <v>META</v>
       </c>
       <c r="B4">
-        <v>99.20780205009382</v>
+        <v>99.22009806722488</v>
       </c>
       <c r="C4">
-        <v>79.7349617912448</v>
+        <v>59.497378817906416</v>
       </c>
       <c r="D4">
-        <v>80.48809578182747</v>
+        <v>71.82444586443386</v>
       </c>
     </row>
     <row r="5">
@@ -1265,10 +1265,10 @@
         <v>100</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>60.200539477765204</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>72.56788595322104</v>
       </c>
     </row>
   </sheetData>
@@ -1361,7 +1361,7 @@
         <v>0.005</v>
       </c>
       <c r="C2">
-        <v>-0.7982260415155573</v>
+        <v>-0.796818046550493</v>
       </c>
       <c r="D2">
         <f>STANDARDIZE(0.005,AVERAGE('Sector Reference'!C:C),STDEV('Sector Reference'!C:C))</f>
@@ -1385,22 +1385,22 @@
         <f>STANDARDIZE(8.254,AVERAGE('Sector Reference'!E:E),STDEV('Sector Reference'!E:E))</f>
       </c>
       <c r="K2">
-        <v>18.301338</v>
+        <v>19.266619</v>
       </c>
       <c r="L2">
-        <v>-0.1541075049850813</v>
+        <v>-0.1167099790135547</v>
       </c>
       <c r="M2">
-        <f>STANDARDIZE(18.301338,AVERAGE('Sector Reference'!F:F),STDEV('Sector Reference'!F:F))</f>
+        <f>STANDARDIZE(19.266619,AVERAGE('Sector Reference'!F:F),STDEV('Sector Reference'!F:F))</f>
       </c>
       <c r="N2">
-        <v>0.20801738710456422</v>
+        <v>0.023426486394750368</v>
       </c>
       <c r="O2">
-        <v>1.1672362460236527</v>
+        <v>1.6974665331641425</v>
       </c>
       <c r="P2">
-        <f>STANDARDIZE(0.20801738710456422,AVERAGE('Sector Reference'!G:G),STDEV('Sector Reference'!G:G))</f>
+        <f>STANDARDIZE(0.023426486394750368,AVERAGE('Sector Reference'!G:G),STDEV('Sector Reference'!G:G))</f>
       </c>
     </row>
     <row r="3">
@@ -1408,13 +1408,13 @@
         <v>AAPL</v>
       </c>
       <c r="B3">
-        <v>0.005</v>
+        <v>0.0050999997</v>
       </c>
       <c r="C3">
-        <v>-0.7982260415155573</v>
+        <v>-0.7913866647836603</v>
       </c>
       <c r="D3">
-        <f>STANDARDIZE(0.005,AVERAGE('Sector Reference'!C:C),STDEV('Sector Reference'!C:C))</f>
+        <f>STANDARDIZE(0.0050999997,AVERAGE('Sector Reference'!C:C),STDEV('Sector Reference'!C:C))</f>
       </c>
       <c r="E3">
         <v>0.24301</v>
@@ -1435,22 +1435,22 @@
         <f>STANDARDIZE(146.994,AVERAGE('Sector Reference'!E:E),STDEV('Sector Reference'!E:E))</f>
       </c>
       <c r="K3">
-        <v>24.892899</v>
+        <v>24.338146</v>
       </c>
       <c r="L3">
-        <v>0.058985927120379436</v>
+        <v>0.04976935637150137</v>
       </c>
       <c r="M3">
-        <f>STANDARDIZE(24.892899,AVERAGE('Sector Reference'!F:F),STDEV('Sector Reference'!F:F))</f>
+        <f>STANDARDIZE(24.338146,AVERAGE('Sector Reference'!F:F),STDEV('Sector Reference'!F:F))</f>
       </c>
       <c r="N3">
-        <v>0.20469050365244137</v>
+        <v>0.0007899811224648264</v>
       </c>
       <c r="O3">
-        <v>1.12736490870808</v>
+        <v>-1.2562608084210165</v>
       </c>
       <c r="P3">
-        <f>STANDARDIZE(0.20469050365244137,AVERAGE('Sector Reference'!G:G),STDEV('Sector Reference'!G:G))</f>
+        <f>STANDARDIZE(0.0007899811224648264,AVERAGE('Sector Reference'!G:G),STDEV('Sector Reference'!G:G))</f>
       </c>
     </row>
     <row r="4">
@@ -1461,7 +1461,7 @@
         <v>0.0033000002</v>
       </c>
       <c r="C4">
-        <v>-0.8933156128261037</v>
+        <v>-0.8891518027251564</v>
       </c>
       <c r="D4">
         <f>STANDARDIZE(0.0033000002,AVERAGE('Sector Reference'!C:C),STDEV('Sector Reference'!C:C))</f>
@@ -1485,22 +1485,22 @@
         <f>STANDARDIZE(26.763,AVERAGE('Sector Reference'!E:E),STDEV('Sector Reference'!E:E))</f>
       </c>
       <c r="K4">
-        <v>25.181818</v>
+        <v>25.276854</v>
       </c>
       <c r="L4">
-        <v>0.06832616402488166</v>
+        <v>0.08058364247520063</v>
       </c>
       <c r="M4">
-        <f>STANDARDIZE(25.181818,AVERAGE('Sector Reference'!F:F),STDEV('Sector Reference'!F:F))</f>
+        <f>STANDARDIZE(25.276854,AVERAGE('Sector Reference'!F:F),STDEV('Sector Reference'!F:F))</f>
       </c>
       <c r="N4">
-        <v>0.14011148452578578</v>
+        <v>0.005807474659536062</v>
       </c>
       <c r="O4">
-        <v>0.3534117804538478</v>
+        <v>-0.6015525101034744</v>
       </c>
       <c r="P4">
-        <f>STANDARDIZE(0.14011148452578578,AVERAGE('Sector Reference'!G:G),STDEV('Sector Reference'!G:G))</f>
+        <f>STANDARDIZE(0.005807474659536062,AVERAGE('Sector Reference'!G:G),STDEV('Sector Reference'!G:G))</f>
       </c>
     </row>
     <row r="5">
@@ -1508,13 +1508,13 @@
         <v>MSFT</v>
       </c>
       <c r="B5">
-        <v>0.0072000003</v>
+        <v>0.0073</v>
       </c>
       <c r="C5">
-        <v>-0.6751689179734995</v>
+        <v>-0.6718958911468715</v>
       </c>
       <c r="D5">
-        <f>STANDARDIZE(0.0072000003,AVERAGE('Sector Reference'!C:C),STDEV('Sector Reference'!C:C))</f>
+        <f>STANDARDIZE(0.0073,AVERAGE('Sector Reference'!C:C),STDEV('Sector Reference'!C:C))</f>
       </c>
       <c r="E5">
         <v>0.35789</v>
@@ -1535,22 +1535,22 @@
         <f>STANDARDIZE(32.626,AVERAGE('Sector Reference'!E:E),STDEV('Sector Reference'!E:E))</f>
       </c>
       <c r="K5">
-        <v>30.646824</v>
+        <v>30.535118</v>
       </c>
       <c r="L5">
-        <v>0.2450000785979146</v>
+        <v>0.2531928578060402</v>
       </c>
       <c r="M5">
-        <f>STANDARDIZE(30.646824,AVERAGE('Sector Reference'!F:F),STDEV('Sector Reference'!F:F))</f>
+        <f>STANDARDIZE(30.535118,AVERAGE('Sector Reference'!F:F),STDEV('Sector Reference'!F:F))</f>
       </c>
       <c r="N5">
-        <v>0.021735881285363523</v>
+        <v>0.008136970526567382</v>
       </c>
       <c r="O5">
-        <v>-1.0652714029686576</v>
+        <v>-0.29758793819650925</v>
       </c>
       <c r="P5">
-        <f>STANDARDIZE(0.021735881285363523,AVERAGE('Sector Reference'!G:G),STDEV('Sector Reference'!G:G))</f>
+        <f>STANDARDIZE(0.008136970526567382,AVERAGE('Sector Reference'!G:G),STDEV('Sector Reference'!G:G))</f>
       </c>
     </row>
   </sheetData>

</xml_diff>